<commit_message>
feat: Se agrego tabla de registro de tablas obtenidas de la API
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B45F2A32-9AE3-4366-BDDB-DAA6DF042E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601E3A0-D007-4B68-A8FD-1C83CDA0BB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>mal_id</t>
   </si>
@@ -246,6 +246,9 @@
     <t>Miembros</t>
   </si>
   <si>
+    <t>popularidad</t>
+  </si>
+  <si>
     <t>populariadad</t>
   </si>
   <si>
@@ -256,13 +259,28 @@
   </si>
   <si>
     <t>anime_rank</t>
+  </si>
+  <si>
+    <t>Tablas Extraidas de la API</t>
+  </si>
+  <si>
+    <t>Nombre tabla</t>
+  </si>
+  <si>
+    <t>Extraida</t>
+  </si>
+  <si>
+    <t>generos</t>
+  </si>
+  <si>
+    <t>anime_genero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +307,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,6 +467,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,6 +507,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,15 +823,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FCF1D3-887E-4AC0-9837-DB93C9FF74EE}">
-  <dimension ref="B3:P23"/>
+  <dimension ref="B3:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -816,52 +850,52 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="7"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="9"/>
       <c r="N3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="2:16" s="8" customFormat="1">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:16" s="10" customFormat="1">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -872,7 +906,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -881,25 +915,25 @@
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -913,7 +947,7 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -922,7 +956,7 @@
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="12" t="s">
         <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -931,10 +965,10 @@
       <c r="L6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -967,10 +1001,10 @@
       <c r="L7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="20" t="s">
         <v>15</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -994,12 +1028,12 @@
         <v>22</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="20" t="s">
         <v>13</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1016,10 +1050,10 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="21" t="s">
         <v>14</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -1036,10 +1070,10 @@
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O10" s="19" t="s">
+      <c r="N10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -1054,19 +1088,19 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="17" t="s">
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="1" t="s">
@@ -1078,16 +1112,16 @@
       <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1150,7 +1184,7 @@
     </row>
     <row r="16" spans="2:16">
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1159,13 +1193,63 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+    <row r="21" spans="2:5">
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="22"/>
       <c r="D23" s="5"/>
     </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="E30" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="F3:H3"/>

</xml_diff>

<commit_message>
feat: Se marcaron las tablas que ya se extrago la información
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601E3A0-D007-4B68-A8FD-1C83CDA0BB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CBE460-6299-44BE-97AC-AC0B0015A64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>mal_id</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>anime_genero</t>
+  </si>
+  <si>
+    <t>Si</t>
   </si>
 </sst>
 </file>
@@ -507,8 +510,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,7 +829,7 @@
   <dimension ref="B3:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1211,26 +1214,32 @@
       <c r="B23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="23"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
@@ -1245,7 +1254,7 @@
       <c r="C28" s="1"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="E30" s="23"/>
+      <c r="E30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
feat: Se marco casilla de tabla extraidas popularidad
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CBE460-6299-44BE-97AC-AC0B0015A64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B326D9-9943-460D-8CA5-84B033CA71F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
   <si>
     <t>mal_id</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Si</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
@@ -457,53 +460,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,6 +480,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FCF1D3-887E-4AC0-9837-DB93C9FF74EE}">
   <dimension ref="B3:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -843,62 +844,62 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="8" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="J3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="9"/>
-      <c r="N3" s="4" t="s">
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
+      <c r="N3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="2:16" s="10" customFormat="1">
-      <c r="B4" s="11" t="s">
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+    </row>
+    <row r="4" spans="2:16">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -909,7 +910,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -918,7 +919,7 @@
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -927,16 +928,16 @@
       <c r="K5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -950,7 +951,7 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -959,7 +960,7 @@
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -968,10 +969,10 @@
       <c r="L6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -1004,10 +1005,10 @@
       <c r="L7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -1033,10 +1034,10 @@
       <c r="L8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1053,10 +1054,10 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="N9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="O9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -1073,10 +1074,10 @@
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -1093,17 +1094,14 @@
       <c r="D11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="19" t="s">
+      <c r="G11" s="20"/>
+      <c r="I11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="1" t="s">
@@ -1115,16 +1113,16 @@
       <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1197,10 +1195,10 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="1" t="s">
@@ -1211,13 +1209,13 @@
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="1" t="s">
@@ -1239,7 +1237,9 @@
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
@@ -1254,7 +1254,7 @@
       <c r="C28" s="1"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="E30" s="22"/>
+      <c r="E30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
feat: Marcado de casilla de Tablas extraidas
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B326D9-9943-460D-8CA5-84B033CA71F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C1AA08-E900-4444-B04E-4873D1D2CE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>mal_id</t>
   </si>
@@ -830,7 +830,7 @@
   <dimension ref="B3:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1245,7 +1245,9 @@
       <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="1" t="s">

</xml_diff>

<commit_message>
feat: Se marco casilla de anime_studio de tablas extraidas
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C1AA08-E900-4444-B04E-4873D1D2CE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADF1553-3C1F-4CBD-96AF-EBF8099C9856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>mal_id</t>
   </si>
@@ -830,7 +830,7 @@
   <dimension ref="B3:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1253,7 +1253,9 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="30" spans="2:5">
       <c r="E30" s="9"/>

</xml_diff>

<commit_message>
fix: Correción a tipo de datos a tabla de popularidad y estudio
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADF1553-3C1F-4CBD-96AF-EBF8099C9856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759ABF2C-6242-4CC4-B18D-499D6CA7B7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>FLOAT</t>
-  </si>
-  <si>
     <r>
       <t>INT</t>
     </r>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
   <dimension ref="B3:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -923,7 +923,7 @@
         <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>0</v>
@@ -938,12 +938,12 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -952,7 +952,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
@@ -961,7 +961,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>1</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -993,11 +993,11 @@
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="8" spans="2:16">
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -1026,22 +1026,22 @@
         <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -1055,7 +1055,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>14</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1075,7 +1075,7 @@
         <v>33</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>19</v>
@@ -1086,13 +1086,13 @@
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>23</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1140,18 +1140,18 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -1163,18 +1163,18 @@
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:16">
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="16" spans="2:16">
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1196,16 +1196,16 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="12"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -1213,16 +1213,16 @@
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -1230,23 +1230,23 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -1254,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:5">

</xml_diff>

<commit_message>
fix: Corrección al tipo de datos de tabla popularidad
</commit_message>
<xml_diff>
--- a/reports/layout_tablas.xlsx
+++ b/reports/layout_tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\anime_analisis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759ABF2C-6242-4CC4-B18D-499D6CA7B7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25D781-15B1-47CF-9892-375E42991FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
+    <workbookView xWindow="2784" yWindow="516" windowWidth="18420" windowHeight="11136" xr2:uid="{901566D2-B232-4666-944D-8A56552DEA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>mal_id</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>Float</t>
   </si>
 </sst>
 </file>
@@ -326,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +372,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -460,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -474,10 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,6 +518,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FCF1D3-887E-4AC0-9837-DB93C9FF74EE}">
   <dimension ref="B3:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -844,26 +855,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="F3" s="15" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="F3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="J3" s="16" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="N3" s="14" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="N3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="3" t="s">
@@ -904,40 +915,40 @@
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="21" t="s">
         <v>35</v>
       </c>
     </row>
@@ -969,14 +980,14 @@
       <c r="L6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>33</v>
+      <c r="P6" s="20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -996,22 +1007,22 @@
         <v>36</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1034,13 +1045,13 @@
       <c r="L8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1054,33 +1065,33 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1094,14 +1105,14 @@
       <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="I11" s="21" t="s">
+      <c r="G11" s="18"/>
+      <c r="I11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="21"/>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="1" t="s">
@@ -1136,16 +1147,16 @@
       <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="20" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1184,21 +1195,21 @@
       </c>
     </row>
     <row r="16" spans="2:16">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="1" t="s">
@@ -1237,7 +1248,7 @@
       <c r="B26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1258,7 +1269,7 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="E30" s="9"/>
+      <c r="E30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>